<commit_message>
update util with printcount
</commit_message>
<xml_diff>
--- a/packinglist.xlsx
+++ b/packinglist.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Template Backup" sheetId="172" r:id="rId2"/>
     <sheet name="Template (2)" sheetId="23" r:id="rId3"/>
-    <sheet name="print 1" sheetId="222" r:id="rId4"/>
+    <sheet name="print 1" sheetId="234" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -136,22 +136,34 @@
     <t>[billaddress4]</t>
   </si>
   <si>
-    <t>Pcs</t>
-  </si>
-  <si>
-    <t>23-09-2024 00:42</t>
-  </si>
-  <si>
-    <t>Asia Makmur</t>
-  </si>
-  <si>
-    <t>Jl. Raya Bogor KM 31.9 No 16</t>
-  </si>
-  <si>
-    <t>TH-887JG</t>
-  </si>
-  <si>
-    <t>TH-131AA</t>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Jl. Cinere Raya No.202</t>
+  </si>
+  <si>
+    <t>Cinere, Kota Depok</t>
+  </si>
+  <si>
+    <t>Jawa Barat, 16514</t>
+  </si>
+  <si>
+    <t>[reprint]</t>
+  </si>
+  <si>
+    <t>Customer :[count]</t>
+  </si>
+  <si>
+    <t>TFL-138-22</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>TA-1006-KB</t>
+  </si>
+  <si>
+    <t>02-10-2024 06:15</t>
   </si>
 </sst>
 </file>
@@ -554,80 +566,80 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,9 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1501,13 +1511,13 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41" t="s">
@@ -1519,9 +1529,9 @@
       <c r="A2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -1534,19 +1544,19 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="28"/>
@@ -1564,7 +1574,7 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="49" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="5"/>
@@ -1572,7 +1582,9 @@
       <c r="D5" s="5"/>
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="G5" s="42" t="s">
+        <v>26</v>
+      </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -1588,133 +1600,133 @@
       <c r="D6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="38"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="50"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="59"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="69"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="51"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
       <c r="B9" s="25"/>
-      <c r="C9" s="51"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="B10" s="25"/>
-      <c r="C10" s="51"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="51"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="25"/>
-      <c r="C12" s="51"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="62"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="51"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="51"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="62"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="51"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="62"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="62"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="52"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="34"/>
       <c r="G18" s="18" t="s">
         <v>10</v>
@@ -1725,29 +1737,29 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="13"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1779,11 +1791,11 @@
       <c r="A1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41" t="s">
@@ -1795,9 +1807,9 @@
       <c r="A2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -1813,9 +1825,9 @@
       <c r="A3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -1864,11 +1876,11 @@
       <c r="D6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1876,9 +1888,9 @@
       <c r="B7" s="26"/>
       <c r="C7" s="22"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="59"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="69"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1886,9 +1898,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="23"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1896,9 +1908,9 @@
       <c r="B9" s="25"/>
       <c r="C9" s="23"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1906,9 +1918,9 @@
       <c r="B10" s="25"/>
       <c r="C10" s="23"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1916,9 +1928,9 @@
       <c r="B11" s="25"/>
       <c r="C11" s="23"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1926,9 +1938,9 @@
       <c r="B12" s="25"/>
       <c r="C12" s="23"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="62"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1936,9 +1948,9 @@
       <c r="B13" s="25"/>
       <c r="C13" s="23"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1946,9 +1958,9 @@
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="62"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1956,9 +1968,9 @@
       <c r="B15" s="25"/>
       <c r="C15" s="23"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="62"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1966,9 +1978,9 @@
       <c r="B16" s="25"/>
       <c r="C16" s="23"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="62"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1976,21 +1988,21 @@
       <c r="B17" s="27"/>
       <c r="C17" s="24"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="34"/>
       <c r="G18" s="18" t="s">
         <v>10</v>
@@ -2001,20 +2013,14 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="13"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2024,6 +2030,12 @@
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2054,11 +2066,11 @@
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
       <c r="F1" s="32" t="s">
         <v>15</v>
       </c>
@@ -2068,9 +2080,9 @@
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2083,9 +2095,9 @@
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -2126,10 +2138,10 @@
       <c r="C6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="69"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="16" t="s">
         <v>4</v>
       </c>
@@ -2139,8 +2151,8 @@
       <c r="A7" s="19"/>
       <c r="B7" s="26"/>
       <c r="C7" s="22"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="59"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="29"/>
       <c r="G7" s="1"/>
     </row>
@@ -2148,8 +2160,8 @@
       <c r="A8" s="20"/>
       <c r="B8" s="25"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="62"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
     </row>
@@ -2157,8 +2169,8 @@
       <c r="A9" s="20"/>
       <c r="B9" s="25"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="62"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="30"/>
       <c r="G9" s="1"/>
     </row>
@@ -2166,8 +2178,8 @@
       <c r="A10" s="20"/>
       <c r="B10" s="25"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="62"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="30"/>
       <c r="G10" s="1"/>
     </row>
@@ -2175,8 +2187,8 @@
       <c r="A11" s="20"/>
       <c r="B11" s="25"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="62"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="30"/>
       <c r="G11" s="1"/>
     </row>
@@ -2184,8 +2196,8 @@
       <c r="A12" s="20"/>
       <c r="B12" s="25"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="62"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="56"/>
       <c r="F12" s="30"/>
       <c r="G12" s="1"/>
     </row>
@@ -2193,8 +2205,8 @@
       <c r="A13" s="20"/>
       <c r="B13" s="25"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="62"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="30"/>
       <c r="G13" s="1"/>
     </row>
@@ -2202,8 +2214,8 @@
       <c r="A14" s="20"/>
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="62"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="56"/>
       <c r="F14" s="30"/>
       <c r="G14" s="1"/>
     </row>
@@ -2211,8 +2223,8 @@
       <c r="A15" s="20"/>
       <c r="B15" s="25"/>
       <c r="C15" s="23"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="62"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="30"/>
       <c r="G15" s="1"/>
     </row>
@@ -2220,8 +2232,8 @@
       <c r="A16" s="20"/>
       <c r="B16" s="25"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="62"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="56"/>
       <c r="F16" s="30"/>
       <c r="G16" s="1"/>
     </row>
@@ -2229,8 +2241,8 @@
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="65"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="31"/>
       <c r="G17" s="1"/>
     </row>
@@ -2238,12 +2250,12 @@
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
       <c r="F18" s="18" t="s">
         <v>10</v>
       </c>
@@ -2253,19 +2265,13 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2275,6 +2281,12 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2286,9 +2298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2306,11 +2316,11 @@
       <c r="A1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
@@ -2318,11 +2328,11 @@
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+        <v>22</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -2330,24 +2340,26 @@
         <v>16</v>
       </c>
       <c r="G2" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="70"/>
+      <c r="A4" s="49" t="s">
+        <v>24</v>
+      </c>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -2358,12 +2370,14 @@
         <v>16</v>
       </c>
       <c r="G4" s="43">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="70"/>
+      <c r="A5" s="49" t="s">
+        <v>25</v>
+      </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2373,158 +2387,158 @@
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="26">
-        <v>7</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="33"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="59"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="69"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="25">
-        <v>10</v>
-      </c>
-      <c r="C8" s="51" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>29</v>
       </c>
       <c r="D8" s="36"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
       <c r="B9" s="25"/>
-      <c r="C9" s="51"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="B10" s="25"/>
-      <c r="C10" s="51"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="51"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="25"/>
-      <c r="C12" s="51"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="62"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="51"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="51"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="62"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="51"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="62"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="62"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="52"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="47"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="52"/>
       <c r="G18" s="18" t="s">
         <v>10</v>
       </c>
@@ -2534,9 +2548,9 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="46"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="51"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>

</xml_diff>

<commit_message>
add DT as date time when printing
</commit_message>
<xml_diff>
--- a/packinglist.xlsx
+++ b/packinglist.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
   <si>
     <r>
       <rPr>
@@ -165,12 +165,15 @@
   <si>
     <t>02-10-2024 06:15</t>
   </si>
+  <si>
+    <t>[dt]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -232,6 +235,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -427,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -590,6 +599,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -617,29 +647,11 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1495,7 +1507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1513,11 +1527,11 @@
       <c r="A1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41" t="s">
@@ -1529,9 +1543,9 @@
       <c r="A2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -1547,9 +1561,9 @@
       <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -1600,11 +1614,11 @@
       <c r="D6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1612,9 +1626,9 @@
       <c r="B7" s="26"/>
       <c r="C7" s="46"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1622,9 +1636,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="47"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="56"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="63"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1632,9 +1646,9 @@
       <c r="B9" s="25"/>
       <c r="C9" s="47"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="56"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="63"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1642,9 +1656,9 @@
       <c r="B10" s="25"/>
       <c r="C10" s="47"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="63"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1652,9 +1666,9 @@
       <c r="B11" s="25"/>
       <c r="C11" s="47"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="63"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1662,9 +1676,9 @@
       <c r="B12" s="25"/>
       <c r="C12" s="47"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="63"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1672,9 +1686,9 @@
       <c r="B13" s="25"/>
       <c r="C13" s="47"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="56"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="63"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1682,9 +1696,9 @@
       <c r="B14" s="25"/>
       <c r="C14" s="47"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="56"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="63"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1692,9 +1706,9 @@
       <c r="B15" s="25"/>
       <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1702,9 +1716,9 @@
       <c r="B16" s="25"/>
       <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="56"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="63"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1712,54 +1726,54 @@
       <c r="B17" s="27"/>
       <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="59"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="34"/>
-      <c r="G18" s="18" t="s">
-        <v>10</v>
-      </c>
+      <c r="G18" s="18"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="71" t="s">
+        <v>32</v>
+      </c>
       <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
     <mergeCell ref="B1:D3"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B18:E18"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1791,11 +1805,11 @@
       <c r="A1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41" t="s">
@@ -1807,9 +1821,9 @@
       <c r="A2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -1825,9 +1839,9 @@
       <c r="A3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -1876,11 +1890,11 @@
       <c r="D6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1888,9 +1902,9 @@
       <c r="B7" s="26"/>
       <c r="C7" s="22"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1898,9 +1912,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="23"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="56"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="63"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1908,9 +1922,9 @@
       <c r="B9" s="25"/>
       <c r="C9" s="23"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="56"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="63"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1918,9 +1932,9 @@
       <c r="B10" s="25"/>
       <c r="C10" s="23"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="63"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1928,9 +1942,9 @@
       <c r="B11" s="25"/>
       <c r="C11" s="23"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="63"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1938,9 +1952,9 @@
       <c r="B12" s="25"/>
       <c r="C12" s="23"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="63"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1948,9 +1962,9 @@
       <c r="B13" s="25"/>
       <c r="C13" s="23"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="56"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="63"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1958,9 +1972,9 @@
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="56"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="63"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1968,9 +1982,9 @@
       <c r="B15" s="25"/>
       <c r="C15" s="23"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1978,9 +1992,9 @@
       <c r="B16" s="25"/>
       <c r="C16" s="23"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="56"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="63"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1988,21 +2002,21 @@
       <c r="B17" s="27"/>
       <c r="C17" s="24"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="59"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="34"/>
       <c r="G18" s="18" t="s">
         <v>10</v>
@@ -2013,14 +2027,20 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="13"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2030,12 +2050,6 @@
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2066,11 +2080,11 @@
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
       <c r="F1" s="32" t="s">
         <v>15</v>
       </c>
@@ -2080,9 +2094,9 @@
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2095,9 +2109,9 @@
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -2151,8 +2165,8 @@
       <c r="A7" s="19"/>
       <c r="B7" s="26"/>
       <c r="C7" s="22"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="69"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="60"/>
       <c r="F7" s="29"/>
       <c r="G7" s="1"/>
     </row>
@@ -2160,8 +2174,8 @@
       <c r="A8" s="20"/>
       <c r="B8" s="25"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="56"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
     </row>
@@ -2169,8 +2183,8 @@
       <c r="A9" s="20"/>
       <c r="B9" s="25"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="56"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="30"/>
       <c r="G9" s="1"/>
     </row>
@@ -2178,8 +2192,8 @@
       <c r="A10" s="20"/>
       <c r="B10" s="25"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="56"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="30"/>
       <c r="G10" s="1"/>
     </row>
@@ -2187,8 +2201,8 @@
       <c r="A11" s="20"/>
       <c r="B11" s="25"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="56"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="63"/>
       <c r="F11" s="30"/>
       <c r="G11" s="1"/>
     </row>
@@ -2196,8 +2210,8 @@
       <c r="A12" s="20"/>
       <c r="B12" s="25"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="56"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="63"/>
       <c r="F12" s="30"/>
       <c r="G12" s="1"/>
     </row>
@@ -2205,8 +2219,8 @@
       <c r="A13" s="20"/>
       <c r="B13" s="25"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="56"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="63"/>
       <c r="F13" s="30"/>
       <c r="G13" s="1"/>
     </row>
@@ -2214,8 +2228,8 @@
       <c r="A14" s="20"/>
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="56"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="63"/>
       <c r="F14" s="30"/>
       <c r="G14" s="1"/>
     </row>
@@ -2223,8 +2237,8 @@
       <c r="A15" s="20"/>
       <c r="B15" s="25"/>
       <c r="C15" s="23"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="56"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="63"/>
       <c r="F15" s="30"/>
       <c r="G15" s="1"/>
     </row>
@@ -2232,8 +2246,8 @@
       <c r="A16" s="20"/>
       <c r="B16" s="25"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="56"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="63"/>
       <c r="F16" s="30"/>
       <c r="G16" s="1"/>
     </row>
@@ -2241,8 +2255,8 @@
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="59"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="66"/>
       <c r="F17" s="31"/>
       <c r="G17" s="1"/>
     </row>
@@ -2250,12 +2264,12 @@
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
       <c r="F18" s="18" t="s">
         <v>10</v>
       </c>
@@ -2265,13 +2279,19 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2281,12 +2301,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2316,11 +2330,11 @@
       <c r="A1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
@@ -2330,9 +2344,9 @@
       <c r="A2" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -2348,9 +2362,9 @@
       <c r="A3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -2399,11 +2413,11 @@
       <c r="D6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2417,9 +2431,9 @@
         <v>29</v>
       </c>
       <c r="D7" s="33"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2433,9 +2447,9 @@
         <v>29</v>
       </c>
       <c r="D8" s="36"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="56"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="63"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2443,9 +2457,9 @@
       <c r="B9" s="25"/>
       <c r="C9" s="47"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="56"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="63"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2453,9 +2467,9 @@
       <c r="B10" s="25"/>
       <c r="C10" s="47"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="63"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2463,9 +2477,9 @@
       <c r="B11" s="25"/>
       <c r="C11" s="47"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="63"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2473,9 +2487,9 @@
       <c r="B12" s="25"/>
       <c r="C12" s="47"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="63"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2483,9 +2497,9 @@
       <c r="B13" s="25"/>
       <c r="C13" s="47"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="56"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="63"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2493,9 +2507,9 @@
       <c r="B14" s="25"/>
       <c r="C14" s="47"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="56"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="63"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2503,9 +2517,9 @@
       <c r="B15" s="25"/>
       <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2513,9 +2527,9 @@
       <c r="B16" s="25"/>
       <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="56"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="63"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2523,21 +2537,21 @@
       <c r="B17" s="27"/>
       <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="59"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="52"/>
       <c r="G18" s="18" t="s">
         <v>10</v>
@@ -2548,14 +2562,20 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="51"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2565,12 +2585,6 @@
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update add batch for ALL branch
</commit_message>
<xml_diff>
--- a/packinglist.xlsx
+++ b/packinglist.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sugi\Documents\Python Projects\DBW\PrintServerDasa\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18912" windowHeight="8868"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18915" windowHeight="8865" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Template Backup" sheetId="249" r:id="rId2"/>
     <sheet name="Template old" sheetId="172" r:id="rId3"/>
     <sheet name="Template (2)" sheetId="23" r:id="rId4"/>
-    <sheet name="print 1" sheetId="248" r:id="rId5"/>
+    <sheet name="print 1" sheetId="281" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
   <si>
     <r>
       <rPr>
@@ -155,44 +150,32 @@
     <t>[shiptoval]</t>
   </si>
   <si>
-    <t>CV. Kuning Express</t>
-  </si>
-  <si>
-    <t>JL. Urip Sumoharjo RT.001 RW.001</t>
-  </si>
-  <si>
-    <t>Beru Wlingi</t>
-  </si>
-  <si>
-    <t>Blitar</t>
-  </si>
-  <si>
-    <t>Re-Print</t>
-  </si>
-  <si>
-    <t>TH-001AA</t>
-  </si>
-  <si>
     <t>Pcs</t>
   </si>
   <si>
-    <t>15-06-2025 20:36</t>
-  </si>
-  <si>
-    <t>ShipTo</t>
-  </si>
-  <si>
-    <t>Merdeka</t>
-  </si>
-  <si>
-    <t>Customer :..</t>
+    <t>Abdilla, UD</t>
+  </si>
+  <si>
+    <t>JL. Letjen Sutoyo No.18</t>
+  </si>
+  <si>
+    <t>Burengan, Kec. Pesantren</t>
+  </si>
+  <si>
+    <t>Kota Kediri</t>
+  </si>
+  <si>
+    <t>21-07-2025 15:50</t>
+  </si>
+  <si>
+    <t>ECO-SLD011G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -255,12 +238,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -461,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -612,74 +589,80 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1263,7 +1246,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="95250" y="4023359"/>
+          <a:off x="95250" y="4057649"/>
           <a:ext cx="1790700" cy="45719"/>
         </a:xfrm>
         <a:custGeom>
@@ -1307,7 +1290,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2846070" y="4032884"/>
+          <a:off x="2486025" y="4067174"/>
           <a:ext cx="1790700" cy="45719"/>
         </a:xfrm>
         <a:custGeom>
@@ -1351,7 +1334,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5511165" y="4023359"/>
+          <a:off x="4648200" y="4057649"/>
           <a:ext cx="1619250" cy="45719"/>
         </a:xfrm>
         <a:custGeom>
@@ -1426,7 +1409,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1458,10 +1441,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1493,7 +1475,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1669,34 +1650,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41" t="s">
@@ -1704,13 +1685,13 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -1722,13 +1703,13 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75">
       <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="42" t="s">
         <v>26</v>
       </c>
@@ -1738,7 +1719,7 @@
       </c>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.75">
       <c r="A4" s="49" t="s">
         <v>20</v>
       </c>
@@ -1756,7 +1737,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.75">
       <c r="A5" s="49" t="s">
         <v>21</v>
       </c>
@@ -1770,7 +1751,7 @@
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="21" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>1</v>
       </c>
@@ -1780,722 +1761,164 @@
       <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="38"/>
       <c r="B7" s="26"/>
       <c r="C7" s="46"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="64"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="20"/>
       <c r="B8" s="25"/>
       <c r="C8" s="47"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="57"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="67"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="20"/>
       <c r="B9" s="25"/>
       <c r="C9" s="47"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="20"/>
       <c r="B10" s="25"/>
       <c r="C10" s="47"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="67"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="20"/>
       <c r="B11" s="25"/>
       <c r="C11" s="47"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="20"/>
       <c r="B12" s="25"/>
       <c r="C12" s="47"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="57"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75">
       <c r="A13" s="20"/>
       <c r="B13" s="25"/>
       <c r="C13" s="47"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75">
       <c r="A14" s="20"/>
       <c r="B14" s="25"/>
       <c r="C14" s="47"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="67"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75">
       <c r="A15" s="20"/>
       <c r="B15" s="25"/>
       <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="20"/>
       <c r="B16" s="25"/>
       <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75">
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
       <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="60"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="63"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="73"/>
       <c r="F18" s="34"/>
       <c r="G18" s="18"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="72" t="s">
+      <c r="G19" s="57" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B18:E18"/>
-  </mergeCells>
-  <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-  </mergeCells>
-  <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E10:G10"/>
     <mergeCell ref="B1:D3"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
@@ -2508,18 +1931,576 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A1" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A2" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75">
+      <c r="A3" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.75">
+      <c r="A4" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.75">
+      <c r="A5" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1">
+      <c r="A6" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75">
+      <c r="A7" s="38"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75">
+      <c r="A8" s="20"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75">
+      <c r="A9" s="20"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75">
+      <c r="A10" s="20"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75">
+      <c r="A11" s="20"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75">
+      <c r="A12" s="20"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75">
+      <c r="A13" s="20"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75">
+      <c r="A14" s="20"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75">
+      <c r="A15" s="20"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75">
+      <c r="A16" s="20"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75">
+      <c r="A17" s="21"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+  </mergeCells>
+  <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A1" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A2" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75">
+      <c r="A3" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.75">
+      <c r="A4" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.75">
+      <c r="A5" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1">
+      <c r="A6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75">
+      <c r="A7" s="38"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75">
+      <c r="A8" s="20"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75">
+      <c r="A9" s="20"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75">
+      <c r="A10" s="20"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75">
+      <c r="A11" s="20"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75">
+      <c r="A12" s="20"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75">
+      <c r="A13" s="20"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75">
+      <c r="A14" s="20"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75">
+      <c r="A15" s="20"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75">
+      <c r="A16" s="20"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75">
+      <c r="A17" s="21"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+  </mergeCells>
+  <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
@@ -2527,27 +2508,27 @@
     <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
       <c r="F1" s="32" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2556,18 +2537,18 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2582,7 +2563,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -2593,7 +2574,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="21" customHeight="1">
       <c r="A6" s="16" t="s">
         <v>1</v>
       </c>
@@ -2603,140 +2584,146 @@
       <c r="C6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="74"/>
       <c r="F6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="19"/>
       <c r="B7" s="26"/>
       <c r="C7" s="22"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="70"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="64"/>
       <c r="F7" s="29"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="20"/>
       <c r="B8" s="25"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="57"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="67"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="20"/>
       <c r="B9" s="25"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="30"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="20"/>
       <c r="B10" s="25"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="67"/>
       <c r="F10" s="30"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75">
       <c r="A11" s="20"/>
       <c r="B11" s="25"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="57"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="67"/>
       <c r="F11" s="30"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75">
       <c r="A12" s="20"/>
       <c r="B12" s="25"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="57"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="67"/>
       <c r="F12" s="30"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75">
       <c r="A13" s="20"/>
       <c r="B13" s="25"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="57"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="30"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75">
       <c r="A14" s="20"/>
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="57"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="30"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75">
       <c r="A15" s="20"/>
       <c r="B15" s="25"/>
       <c r="C15" s="23"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="57"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="30"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75">
       <c r="A16" s="20"/>
       <c r="B16" s="25"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="57"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="67"/>
       <c r="F16" s="30"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75">
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="60"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="31"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
       <c r="F18" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2746,12 +2733,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2760,46 +2741,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
+        <v>29</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -2807,29 +2788,25 @@
         <v>16</v>
       </c>
       <c r="G2" s="45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75">
       <c r="A3" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="42" t="s">
-        <v>36</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="42"/>
-      <c r="G3" s="42" t="s">
-        <v>37</v>
-      </c>
+      <c r="G3" s="42"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.75">
       <c r="A4" s="49" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -2841,183 +2818,181 @@
         <v>16</v>
       </c>
       <c r="G4" s="43">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.75">
       <c r="A5" s="49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
-      <c r="G5" s="42" t="s">
-        <v>32</v>
-      </c>
+      <c r="G5" s="42"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+    <row r="6" spans="1:8" ht="21" customHeight="1">
+      <c r="A6" s="56" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="26">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D7" s="33"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="64"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="20"/>
       <c r="B8" s="25"/>
       <c r="C8" s="47"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="57"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="67"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="20"/>
       <c r="B9" s="25"/>
       <c r="C9" s="47"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="20"/>
       <c r="B10" s="25"/>
       <c r="C10" s="47"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="67"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="20"/>
       <c r="B11" s="25"/>
       <c r="C11" s="47"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="20"/>
       <c r="B12" s="25"/>
       <c r="C12" s="47"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="57"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75">
       <c r="A13" s="20"/>
       <c r="B13" s="25"/>
       <c r="C13" s="47"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75">
       <c r="A14" s="20"/>
       <c r="B14" s="25"/>
       <c r="C14" s="47"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="67"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75">
       <c r="A15" s="20"/>
       <c r="B15" s="25"/>
       <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="20"/>
       <c r="B16" s="25"/>
       <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75">
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
       <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="60"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="53"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="55"/>
       <c r="G18" s="18"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="50">
-        <v>2506161457</v>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="57">
+        <v>2507211550</v>
       </c>
       <c r="H19" s="1"/>
     </row>

</xml_diff>

<commit_message>
add loguru fix printing twice
</commit_message>
<xml_diff>
--- a/packinglist.xlsx
+++ b/packinglist.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18915" windowHeight="8865" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18915" windowHeight="8865"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Template Backup" sheetId="249" r:id="rId2"/>
     <sheet name="Template old" sheetId="172" r:id="rId3"/>
     <sheet name="Template (2)" sheetId="23" r:id="rId4"/>
-    <sheet name="print 1" sheetId="281" r:id="rId5"/>
+    <sheet name="print 1" sheetId="397" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -153,22 +153,43 @@
     <t>Pcs</t>
   </si>
   <si>
-    <t>Abdilla, UD</t>
-  </si>
-  <si>
-    <t>JL. Letjen Sutoyo No.18</t>
-  </si>
-  <si>
-    <t>Burengan, Kec. Pesantren</t>
-  </si>
-  <si>
-    <t>Kota Kediri</t>
-  </si>
-  <si>
-    <t>21-07-2025 15:50</t>
-  </si>
-  <si>
-    <t>ECO-SLD011G</t>
+    <t>Re-Print</t>
+  </si>
+  <si>
+    <t>13-09-2025 13:23</t>
+  </si>
+  <si>
+    <t>Lancar</t>
+  </si>
+  <si>
+    <t>TH-172GL</t>
+  </si>
+  <si>
+    <t>TH-1230GL</t>
+  </si>
+  <si>
+    <t>TH-204GL</t>
+  </si>
+  <si>
+    <t>TH-887JG</t>
+  </si>
+  <si>
+    <t>TH-028G</t>
+  </si>
+  <si>
+    <t>TH-011G</t>
+  </si>
+  <si>
+    <t>TH-171GL</t>
+  </si>
+  <si>
+    <t>PETI</t>
+  </si>
+  <si>
+    <t>0; 40.000</t>
+  </si>
+  <si>
+    <t>Customer :..............</t>
   </si>
 </sst>
 </file>
@@ -601,6 +622,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -610,8 +634,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -633,33 +681,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -744,50 +765,6 @@
         <a:xfrm>
           <a:off x="2486025" y="4067174"/>
           <a:ext cx="1790700" cy="45719"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path w="1371600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="1371600" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:ln w="12192">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1619250" cy="45719"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Shape 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4543425" y="4057649"/>
-          <a:ext cx="1619250" cy="45719"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1319,50 +1296,44 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1619250" cy="45719"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Shape 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="qrSVG" descr="qr0.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4648200" y="4057649"/>
-          <a:ext cx="1619250" cy="45719"/>
+          <a:off x="4886325" y="3467100"/>
+          <a:ext cx="828675" cy="828675"/>
         </a:xfrm>
-        <a:custGeom>
+        <a:prstGeom prst="rect">
           <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path w="1371600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="1371600" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:ln w="12192">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-        </a:ln>
+        </a:prstGeom>
       </xdr:spPr>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1651,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1673,11 +1644,11 @@
       <c r="A1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41" t="s">
@@ -1689,9 +1660,9 @@
       <c r="A2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -1707,9 +1678,9 @@
       <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="42" t="s">
         <v>26</v>
       </c>
@@ -1764,11 +1735,11 @@
       <c r="D6" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75">
@@ -1776,9 +1747,9 @@
       <c r="B7" s="26"/>
       <c r="C7" s="46"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="73"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75">
@@ -1786,9 +1757,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="47"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75">
@@ -1796,9 +1767,9 @@
       <c r="B9" s="25"/>
       <c r="C9" s="47"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75">
@@ -1806,9 +1777,9 @@
       <c r="B10" s="25"/>
       <c r="C10" s="47"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="67"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75">
@@ -1816,9 +1787,9 @@
       <c r="B11" s="25"/>
       <c r="C11" s="47"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="67"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75">
@@ -1826,9 +1797,9 @@
       <c r="B12" s="25"/>
       <c r="C12" s="47"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="67"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75">
@@ -1836,9 +1807,9 @@
       <c r="B13" s="25"/>
       <c r="C13" s="47"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75">
@@ -1846,9 +1817,9 @@
       <c r="B14" s="25"/>
       <c r="C14" s="47"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="67"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
@@ -1856,9 +1827,9 @@
       <c r="B15" s="25"/>
       <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -1866,9 +1837,9 @@
       <c r="B16" s="25"/>
       <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="67"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75">
@@ -1876,21 +1847,21 @@
       <c r="B17" s="27"/>
       <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="73"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
       <c r="F18" s="34"/>
       <c r="G18" s="18"/>
       <c r="H18" s="1"/>
@@ -1899,31 +1870,32 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="57" t="s">
+      <c r="G19" s="54" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="1"/>
     </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1955,11 +1927,11 @@
       <c r="A1" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41" t="s">
@@ -1971,9 +1943,9 @@
       <c r="A2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -1989,9 +1961,9 @@
       <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="42" t="s">
         <v>26</v>
       </c>
@@ -2046,11 +2018,11 @@
       <c r="D6" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75">
@@ -2058,9 +2030,9 @@
       <c r="B7" s="26"/>
       <c r="C7" s="46"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="73"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75">
@@ -2068,9 +2040,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="47"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75">
@@ -2078,9 +2050,9 @@
       <c r="B9" s="25"/>
       <c r="C9" s="47"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75">
@@ -2088,9 +2060,9 @@
       <c r="B10" s="25"/>
       <c r="C10" s="47"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="67"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75">
@@ -2098,9 +2070,9 @@
       <c r="B11" s="25"/>
       <c r="C11" s="47"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="67"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75">
@@ -2108,9 +2080,9 @@
       <c r="B12" s="25"/>
       <c r="C12" s="47"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="67"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75">
@@ -2118,9 +2090,9 @@
       <c r="B13" s="25"/>
       <c r="C13" s="47"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75">
@@ -2128,9 +2100,9 @@
       <c r="B14" s="25"/>
       <c r="C14" s="47"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="67"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
@@ -2138,9 +2110,9 @@
       <c r="B15" s="25"/>
       <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -2148,9 +2120,9 @@
       <c r="B16" s="25"/>
       <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="67"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75">
@@ -2158,21 +2130,21 @@
       <c r="B17" s="27"/>
       <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="73"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
       <c r="F18" s="52"/>
       <c r="G18" s="18"/>
       <c r="H18" s="1"/>
@@ -2181,22 +2153,16 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
       <c r="F19" s="51"/>
-      <c r="G19" s="57" t="s">
+      <c r="G19" s="54" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2206,6 +2172,12 @@
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2237,11 +2209,11 @@
       <c r="A1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41" t="s">
@@ -2253,9 +2225,9 @@
       <c r="A2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -2271,9 +2243,9 @@
       <c r="A3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -2322,11 +2294,11 @@
       <c r="D6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75">
@@ -2334,9 +2306,9 @@
       <c r="B7" s="26"/>
       <c r="C7" s="22"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="73"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75">
@@ -2344,9 +2316,9 @@
       <c r="B8" s="25"/>
       <c r="C8" s="23"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75">
@@ -2354,9 +2326,9 @@
       <c r="B9" s="25"/>
       <c r="C9" s="23"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75">
@@ -2364,9 +2336,9 @@
       <c r="B10" s="25"/>
       <c r="C10" s="23"/>
       <c r="D10" s="36"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="67"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75">
@@ -2374,9 +2346,9 @@
       <c r="B11" s="25"/>
       <c r="C11" s="23"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="67"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75">
@@ -2384,9 +2356,9 @@
       <c r="B12" s="25"/>
       <c r="C12" s="23"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="67"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75">
@@ -2394,9 +2366,9 @@
       <c r="B13" s="25"/>
       <c r="C13" s="23"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75">
@@ -2404,9 +2376,9 @@
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
       <c r="D14" s="36"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="67"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
@@ -2414,9 +2386,9 @@
       <c r="B15" s="25"/>
       <c r="C15" s="23"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -2424,9 +2396,9 @@
       <c r="B16" s="25"/>
       <c r="C16" s="23"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="67"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75">
@@ -2434,21 +2406,21 @@
       <c r="B17" s="27"/>
       <c r="C17" s="24"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="73"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
       <c r="F18" s="34"/>
       <c r="G18" s="18" t="s">
         <v>10</v>
@@ -2459,20 +2431,14 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
       <c r="F19" s="13"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2482,6 +2448,12 @@
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2512,11 +2484,11 @@
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
       <c r="F1" s="32" t="s">
         <v>15</v>
       </c>
@@ -2526,9 +2498,9 @@
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2541,9 +2513,9 @@
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -2597,8 +2569,8 @@
       <c r="A7" s="19"/>
       <c r="B7" s="26"/>
       <c r="C7" s="22"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="64"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="73"/>
       <c r="F7" s="29"/>
       <c r="G7" s="1"/>
     </row>
@@ -2606,8 +2578,8 @@
       <c r="A8" s="20"/>
       <c r="B8" s="25"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="67"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="60"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
     </row>
@@ -2615,8 +2587,8 @@
       <c r="A9" s="20"/>
       <c r="B9" s="25"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="67"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="30"/>
       <c r="G9" s="1"/>
     </row>
@@ -2624,8 +2596,8 @@
       <c r="A10" s="20"/>
       <c r="B10" s="25"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="67"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="60"/>
       <c r="F10" s="30"/>
       <c r="G10" s="1"/>
     </row>
@@ -2633,8 +2605,8 @@
       <c r="A11" s="20"/>
       <c r="B11" s="25"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="67"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="30"/>
       <c r="G11" s="1"/>
     </row>
@@ -2642,8 +2614,8 @@
       <c r="A12" s="20"/>
       <c r="B12" s="25"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="67"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="60"/>
       <c r="F12" s="30"/>
       <c r="G12" s="1"/>
     </row>
@@ -2651,8 +2623,8 @@
       <c r="A13" s="20"/>
       <c r="B13" s="25"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="67"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="60"/>
       <c r="F13" s="30"/>
       <c r="G13" s="1"/>
     </row>
@@ -2660,8 +2632,8 @@
       <c r="A14" s="20"/>
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="67"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="60"/>
       <c r="F14" s="30"/>
       <c r="G14" s="1"/>
     </row>
@@ -2669,8 +2641,8 @@
       <c r="A15" s="20"/>
       <c r="B15" s="25"/>
       <c r="C15" s="23"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="67"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="30"/>
       <c r="G15" s="1"/>
     </row>
@@ -2678,8 +2650,8 @@
       <c r="A16" s="20"/>
       <c r="B16" s="25"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="67"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="60"/>
       <c r="F16" s="30"/>
       <c r="G16" s="1"/>
     </row>
@@ -2687,8 +2659,8 @@
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="70"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="63"/>
       <c r="F17" s="31"/>
       <c r="G17" s="1"/>
     </row>
@@ -2696,12 +2668,12 @@
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
       <c r="F18" s="18" t="s">
         <v>10</v>
       </c>
@@ -2711,19 +2683,13 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2733,6 +2699,12 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2744,8 +2716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2762,13 +2734,13 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="41"/>
@@ -2776,11 +2748,11 @@
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+        <v>31</v>
+      </c>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="42" t="s">
         <v>17</v>
       </c>
@@ -2788,26 +2760,22 @@
         <v>16</v>
       </c>
       <c r="G2" s="45" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75">
-      <c r="A3" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="7" customFormat="1" ht="15.75">
-      <c r="A4" s="49" t="s">
-        <v>31</v>
-      </c>
+      <c r="A4" s="49"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -2818,126 +2786,170 @@
         <v>16</v>
       </c>
       <c r="G4" s="43">
-        <v>102</v>
+        <v>2694</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" ht="15.75">
-      <c r="A5" s="49" t="s">
-        <v>32</v>
-      </c>
+      <c r="A5" s="49"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="G5" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="57" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="57" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="26">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C7" s="46" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="33"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="73"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75">
-      <c r="A8" s="20"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="47"/>
+      <c r="A8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="25">
+        <v>2</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="D8" s="36"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75">
-      <c r="A9" s="20"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="47"/>
+      <c r="A9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="25">
+        <v>2</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" s="36"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75">
-      <c r="A10" s="20"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="47"/>
+      <c r="A10" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="25">
+        <v>2</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="D10" s="36"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="67"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75">
-      <c r="A11" s="20"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="47"/>
+      <c r="A11" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="25">
+        <v>1</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="D11" s="36"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="67"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75">
-      <c r="A12" s="20"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="47"/>
+      <c r="A12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="25">
+        <v>1</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="D12" s="36"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="67"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75">
-      <c r="A13" s="20"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="47"/>
+      <c r="A13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="25">
+        <v>2</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="D13" s="36"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75">
-      <c r="A14" s="20"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="47"/>
+      <c r="A14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="25">
+        <v>1</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="D14" s="36"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="67"/>
+      <c r="E14" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
@@ -2945,9 +2957,9 @@
       <c r="B15" s="25"/>
       <c r="C15" s="47"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -2955,9 +2967,9 @@
       <c r="B16" s="25"/>
       <c r="C16" s="47"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="67"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75">
@@ -2965,22 +2977,22 @@
       <c r="B17" s="27"/>
       <c r="C17" s="48"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="55"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="18"/>
       <c r="H18" s="1"/>
     </row>
@@ -2988,11 +3000,11 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="57">
-        <v>2507211550</v>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="54">
+        <v>2509150724</v>
       </c>
       <c r="H19" s="1"/>
     </row>

</xml_diff>